<commit_message>
make email and evening phone optional
</commit_message>
<xml_diff>
--- a/etc/content.xlsx
+++ b/etc/content.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16729"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkeane\git\pka\etc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <workbookProtection workbookPassword="E35E" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14325"/>
@@ -136,13 +141,13 @@
     <t>2015</t>
   </si>
   <si>
-    <t>Your submission was successful!&lt;br&gt;You will recieve an email shortly.&lt;br&gt;&lt;br&gt;Do you wish to submit again for another child?</t>
+    <t>Your submission was successful!&lt;br&gt;&lt;br&gt;Do you wish to submit again for another child?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -685,6 +690,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -732,7 +740,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -765,9 +773,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -800,6 +825,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">

</xml_diff>

<commit_message>
pka snapshot, form validation and tests
</commit_message>
<xml_diff>
--- a/etc/content.xlsx
+++ b/etc/content.xlsx
@@ -15,7 +15,7 @@
   <sheets>
     <sheet name="content" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>key</t>
   </si>
@@ -90,9 +90,6 @@
     <t>hotline_msg</t>
   </si>
   <si>
-    <t>This form is only a statement of interest and not an application. An Enrollment Specialist will contact you shortly. Please visit &lt;a href="http://nyc.gov/prek" target="_blank"&gt;nyc.gov/prek&lt;/a&gt; for more information.</t>
-  </si>
-  <si>
     <t>form_error</t>
   </si>
   <si>
@@ -108,12 +105,6 @@
     <t>2016-17</t>
   </si>
   <si>
-    <t>&lt;p&gt;The 2016-2017 school year has already begun! &lt;/p&gt;&lt;p&gt; All NYC children born in 2013 will be eligible to attend pre-K in September 2017. &lt;/p&gt;&lt;p&gt;The application for the 2017-2018 school year will open in early 2017.&lt;/p&gt;&lt;p&gt;To ensure that you will be notified about the opening of the application, please click the &amp;#34;&lt;span class="capitalize"&gt;request a call&lt;/span&gt;&amp;#34; button and fill out the Get in Touch form, marking the correct birth year of your child.&lt;/p&gt;&lt;p&gt;If your child was born in 2012 and you have not yet found a pre-K program, please contact the Pre-K Outreach Team at (212) 637-8000 regarding programs that may still have openings.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;All NYC children born in 2012 are eligible to attend pre-K in September 2016.&lt;/p&gt;&lt;p&gt;Click &amp;#34;&lt;span class="capitalize"&gt;request a call&lt;/span&gt;&amp;#34; to hear from an enrollment specialist.&lt;/p&gt;&lt;p&gt;The &lt;span class="capitalize"&gt;main round&lt;/span&gt; application period is now closed. You can still contact &lt;span class="capitalize"&gt;main round&lt;/span&gt; programs directly to inquire about waitlists and availability.&lt;/p&gt;&lt;p&gt;You can still apply for pre-K in the &lt;span class="capitalize"&gt;round 2&lt;/span&gt; application period from June 22-July 10. &lt;span class="capitalize"&gt;round 2&lt;/span&gt; programs include newly awarded NYCEEC pre-k programs&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>Programs that may have immediate availability</t>
   </si>
   <si>
@@ -129,23 +120,38 @@
     <t>Call (212) 637-8000 to contact an enrollment specialist between 9AM-5PM Monday-Friday</t>
   </si>
   <si>
-    <t>http://schools.nyc.gov/OA/SchoolReports/2014-15/School_Quality_Snapshot_2015_HS_${LOCCODE}.pdf</t>
-  </si>
-  <si>
     <t>quality_pdf</t>
   </si>
   <si>
     <t>btn_pdf</t>
   </si>
   <si>
-    <t>quality snapshot</t>
+    <t>Pre-K Snapshot</t>
+  </si>
+  <si>
+    <t>form_invalid</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;The 2016-2017 school year has already begun! &lt;/p&gt;&lt;p&gt; All NYC children born in 2013 will be eligible to attend pre-K in September 2017. &lt;/p&gt;&lt;p&gt;The application for the 2017-2018 school year will open in early 2017.&lt;/p&gt;&lt;p&gt;To ensure that you will be notified about the opening of the application, please click the &amp;#34;&lt;span class='capitalize'&gt;request a call&lt;/span&gt;&amp;#34; button and fill out the Get in Touch form, marking the correct birth year of your child.&lt;/p&gt;&lt;p&gt;If your child was born in 2012 and you have not yet found a pre-K program, please contact the Pre-K Outreach Team at (212) 637-8000 regarding programs that may still have openings.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;All NYC children born in 2012 are eligible to attend pre-K in September 2016.&lt;/p&gt;&lt;p&gt;Click &amp;#34;&lt;span class='capitalize'&gt;request a call&lt;/span&gt;&amp;#34; to hear from an enrollment specialist.&lt;/p&gt;&lt;p&gt;The &lt;span class='capitalize'&gt;main round&lt;/span&gt; application period is now closed. You can still contact &lt;span class='capitalize'&gt;main round&lt;/span&gt; programs directly to inquire about waitlists and availability.&lt;/p&gt;&lt;p&gt;You can still apply for pre-K in the &lt;span class='capitalize'&gt;round 2&lt;/span&gt; application period from June 22-July 10. &lt;span class='capitalize'&gt;round 2&lt;/span&gt; programs include newly awarded NYCEEC pre-k programs&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>This form is only a statement of interest and not an application. An Enrollment Specialist will contact you shortly. Please visit &lt;a href='http://nyc.gov/prek' target='_blank'&gt;nyc.gov/prek&lt;/a&gt; for more information.</t>
+  </si>
+  <si>
+    <t>You have entered invalid information.&lt;p&gt;The form only accepts English language characters.&lt;/p&gt;Please correct the information in the red fields. If you are having difficulty submitting this form, please call 718-935-2009 (Monday-Friday between 8am and 6pm) to speak to a representative.</t>
+  </si>
+  <si>
+    <t>http://schools.nyc.gov/OA/SchoolReports/2014-15/School_Quality_Snapshot_2015_HS_${loccode4}.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,6 +291,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -632,7 +645,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
@@ -646,6 +659,9 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1028,10 +1044,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,7 +1066,7 @@
     </row>
     <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="7">
         <v>2012</v>
@@ -1058,7 +1074,7 @@
     </row>
     <row r="3" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="7">
         <v>2016</v>
@@ -1069,7 +1085,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1093,7 +1109,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1101,7 +1117,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1131,7 +1147,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1139,7 +1155,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1147,7 +1163,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1155,7 +1171,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1163,69 +1179,77 @@
         <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1">
-        <v>2012</v>
+        <v>34</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1">
-        <v>2016</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2016</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>34</v>
+        <v>20</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="FNu/TYOjJKWkslvOw3PqLd3X8FkHOD5vyyicFJaqZ+V+VES3X9pIGgxUKO8kWnUA6+0Rb0kGFmNof9v1UhgVJg==" saltValue="UhEHkWNgGzRM9losmKJ53Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="UMoqmkP41JKp2gMLDb4gibBBWfEmVaIvt67VmL2gEV/EKrZw2zxP0IofdEptLK/IqBPs5N5ohNlxs9oz/4prYg==" saltValue="nbvPSqoMY08tW7Wq8mPhjg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>